<commit_message>
added run with correlation matrix with elections since 1992
</commit_message>
<xml_diff>
--- a/data/states_past_voting.xlsx
+++ b/data/states_past_voting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnrandolph/Desktop/Github/voting-power/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FDC746-03AD-2142-B290-CDC632E197E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971D9EC2-B5C7-7142-91BD-FB4061BBC04E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="22400" xr2:uid="{8FFD2B98-C103-EA40-813B-CD34604588B2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{8FFD2B98-C103-EA40-813B-CD34604588B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -654,9 +654,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90A7799-97B2-6948-81E8-30F265704630}">
   <dimension ref="A1:AC53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A53" sqref="A53"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>